<commit_message>
commit document , mainstoryboard
</commit_message>
<xml_diff>
--- a/Get Photo Facebook/Document/Gui-AppPhotoFB (Autosaved).xlsx
+++ b/Get Photo Facebook/Document/Gui-AppPhotoFB (Autosaved).xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22202"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GUI APP" sheetId="1" r:id="rId1"/>
-    <sheet name="Task Manager" sheetId="2" r:id="rId2"/>
+    <sheet name="issues" sheetId="3" r:id="rId2"/>
+    <sheet name="tasks manager" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
@@ -20,43 +21,139 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>Nhiệm vụ</t>
   </si>
   <si>
-    <t>Task</t>
+    <t>NO.</t>
   </si>
   <si>
-    <t>Duy</t>
+    <t>issues</t>
   </si>
   <si>
-    <t>Quyền</t>
+    <t>description</t>
   </si>
   <si>
-    <t>Monday, 26/6/2017</t>
+    <t>date</t>
   </si>
   <si>
-    <t xml:space="preserve">Design 2 screen Login and Account Infomation </t>
+    <t>resolve solution</t>
   </si>
   <si>
-    <t>(Task)Account information from FB</t>
+    <t xml:space="preserve">commit code between 2 menbers </t>
   </si>
   <si>
-    <t>(Task)Tabbar</t>
+    <t xml:space="preserve"> 2 members create onther folder in project, when merge in code we had error</t>
   </si>
   <si>
-    <t>(Task)Login FB</t>
+    <t>26/06/2017</t>
   </si>
   <si>
-    <t>(Task)Datasource for TableView from FB</t>
+    <t>27/06/2017</t>
+  </si>
+  <si>
+    <t>solution1:delete project and create new one in githud</t>
+  </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>subtasks</t>
+  </si>
+  <si>
+    <t>assignee</t>
+  </si>
+  <si>
+    <t>start date</t>
+  </si>
+  <si>
+    <t>end date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Login</t>
+  </si>
+  <si>
+    <t>create base</t>
+  </si>
+  <si>
+    <t>create stucture project</t>
+  </si>
+  <si>
+    <t>create tabbar Account information &amp; photo</t>
+  </si>
+  <si>
+    <t>use cocoapod add FBSDK</t>
+  </si>
+  <si>
+    <t>import fra to FBSDK.framework</t>
+  </si>
+  <si>
+    <t>design class diagram</t>
+  </si>
+  <si>
+    <t>Design  GUI Login</t>
+  </si>
+  <si>
+    <t>implement Login function</t>
+  </si>
+  <si>
+    <t>Account information</t>
+  </si>
+  <si>
+    <t>design GUI account information</t>
+  </si>
+  <si>
+    <t>get my information</t>
+  </si>
+  <si>
+    <t>get friend information</t>
+  </si>
+  <si>
+    <t>load more friend</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>design GUI photo</t>
+  </si>
+  <si>
+    <t>get list image</t>
+  </si>
+  <si>
+    <t>lazy loading images</t>
+  </si>
+  <si>
+    <t>Photo detail</t>
+  </si>
+  <si>
+    <t>Design GUI photo detail</t>
+  </si>
+  <si>
+    <t>estimation(h)</t>
+  </si>
+  <si>
+    <t>Zoom in/zoom out</t>
+  </si>
+  <si>
+    <t>quyennt</t>
+  </si>
+  <si>
+    <t>duydn</t>
+  </si>
+  <si>
+    <t>quyennt+duydn</t>
+  </si>
+  <si>
+    <t>rotation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,30 +191,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="40"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="25"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,24 +201,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,41 +216,32 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -207,36 +261,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -246,6 +296,10 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -255,6 +309,10 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -376,7 +434,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5006975" y="3362325"/>
+          <a:off x="5006975" y="3425825"/>
           <a:ext cx="1374775" cy="279400"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout2">
@@ -385,8 +443,8 @@
             <a:gd name="adj2" fmla="val 101598"/>
             <a:gd name="adj3" fmla="val 41478"/>
             <a:gd name="adj4" fmla="val 320515"/>
-            <a:gd name="adj5" fmla="val -923864"/>
-            <a:gd name="adj6" fmla="val 320077"/>
+            <a:gd name="adj5" fmla="val 35227"/>
+            <a:gd name="adj6" fmla="val 546405"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -430,8 +488,8 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
@@ -446,8 +504,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10972800" y="371475"/>
-          <a:ext cx="3240000" cy="5760000"/>
+          <a:off x="12496800" y="422275"/>
+          <a:ext cx="3557500" cy="5366300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1888,32 +1946,184 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>29882</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>59764</xdr:rowOff>
+      <xdr:colOff>59764</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>164353</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>74706</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>388469</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>164353</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="66" name="Line Callout 1 65"/>
+        <xdr:cNvPr id="75" name="Rectangle 74"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12526682" y="948764"/>
-          <a:ext cx="3499971" cy="1259542"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout1">
+          <a:off x="12162117" y="5244353"/>
+          <a:ext cx="1673411" cy="478118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Friend</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>433292</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>14942</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>149410</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>149412</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="Rectangle 75"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13880351" y="5214471"/>
+          <a:ext cx="1733177" cy="493059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Photo</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>29883</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="Line Callout 2 80"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14291235" y="5249583"/>
+          <a:ext cx="1750359" cy="548340"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout2">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50682"/>
-            <a:gd name="adj2" fmla="val 101516"/>
-            <a:gd name="adj3" fmla="val 51132"/>
-            <a:gd name="adj4" fmla="val 124404"/>
+            <a:gd name="adj1" fmla="val 51175"/>
+            <a:gd name="adj2" fmla="val 98325"/>
+            <a:gd name="adj3" fmla="val 48859"/>
+            <a:gd name="adj4" fmla="val 167627"/>
+            <a:gd name="adj5" fmla="val 818906"/>
+            <a:gd name="adj6" fmla="val 102074"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -1964,562 +2174,6 @@
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
           </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>29882</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>59763</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>164353</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>164353</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="68" name="Line Callout 1 67"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12526682" y="2548963"/>
-          <a:ext cx="3499971" cy="2593790"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout1">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 25805"/>
-            <a:gd name="adj2" fmla="val 101690"/>
-            <a:gd name="adj3" fmla="val 25440"/>
-            <a:gd name="adj4" fmla="val 125126"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>59764</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>388469</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>164353</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="75" name="Rectangle 74"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12162117" y="5244353"/>
-          <a:ext cx="1673411" cy="478118"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Friend</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>433292</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>14942</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>149410</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>149412</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="76" name="Rectangle 75"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13880351" y="5214471"/>
-          <a:ext cx="1733177" cy="493059"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Photo</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>418353</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>29882</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="77" name="Line Callout 2 76"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12496800" y="5156201"/>
-          <a:ext cx="1764553" cy="563281"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 106681"/>
-            <a:gd name="adj2" fmla="val 49245"/>
-            <a:gd name="adj3" fmla="val 183339"/>
-            <a:gd name="adj4" fmla="val 48109"/>
-            <a:gd name="adj5" fmla="val 184649"/>
-            <a:gd name="adj6" fmla="val 10912"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>448235</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>29883</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>179294</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>44823</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="81" name="Line Callout 2 80"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14291235" y="5186083"/>
-          <a:ext cx="1750359" cy="548340"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 51175"/>
-            <a:gd name="adj2" fmla="val 98325"/>
-            <a:gd name="adj3" fmla="val 48859"/>
-            <a:gd name="adj4" fmla="val 167627"/>
-            <a:gd name="adj5" fmla="val 367270"/>
-            <a:gd name="adj6" fmla="val 166649"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="72" name="Line Callout 2 71"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10642600" y="5867400"/>
-          <a:ext cx="2006600" cy="469900"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 5236"/>
-            <a:gd name="adj2" fmla="val 48629"/>
-            <a:gd name="adj3" fmla="val -1094764"/>
-            <a:gd name="adj4" fmla="val 51055"/>
-            <a:gd name="adj5" fmla="val -1095608"/>
-            <a:gd name="adj6" fmla="val 92574"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(action) go to friend tab</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="78" name="Line Callout 1 77"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8445500" y="304800"/>
-          <a:ext cx="2006600" cy="469900"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout1">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 51182"/>
-            <a:gd name="adj2" fmla="val 101161"/>
-            <a:gd name="adj3" fmla="val 47635"/>
-            <a:gd name="adj4" fmla="val 202806"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(action) login with facebook</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3206,32 +2860,34 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>612587</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>328706</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>44822</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>164352</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>59764</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="158" name="Line Callout 1 157"/>
+        <xdr:cNvPr id="159" name="Line Callout 2 158"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3978087" y="7512422"/>
-          <a:ext cx="3590365" cy="4815542"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout1">
+          <a:off x="3975100" y="7023100"/>
+          <a:ext cx="392206" cy="552822"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout2">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 51093"/>
-            <a:gd name="adj2" fmla="val 100641"/>
-            <a:gd name="adj3" fmla="val 51355"/>
-            <a:gd name="adj4" fmla="val 123237"/>
+            <a:gd name="adj1" fmla="val 4966"/>
+            <a:gd name="adj2" fmla="val 49953"/>
+            <a:gd name="adj3" fmla="val -148136"/>
+            <a:gd name="adj4" fmla="val 54103"/>
+            <a:gd name="adj5" fmla="val 56567"/>
+            <a:gd name="adj6" fmla="val 2156743"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -3282,175 +2938,6 @@
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
           </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>328706</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>44822</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="159" name="Line Callout 2 158"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3975100" y="6959600"/>
-          <a:ext cx="392206" cy="552822"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 4966"/>
-            <a:gd name="adj2" fmla="val 49953"/>
-            <a:gd name="adj3" fmla="val -30974"/>
-            <a:gd name="adj4" fmla="val 54103"/>
-            <a:gd name="adj5" fmla="val -23839"/>
-            <a:gd name="adj6" fmla="val 1334267"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="160" name="Rectangle 159"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8394700" y="9715500"/>
-          <a:ext cx="2006600" cy="749300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(action) zoom in</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(action)zoom out</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4885,15 +4372,15 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12435355" y="7645400"/>
+          <a:off x="12435355" y="7708900"/>
           <a:ext cx="3606239" cy="4193988"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout1">
           <a:avLst>
             <a:gd name="adj1" fmla="val 32730"/>
             <a:gd name="adj2" fmla="val 34"/>
-            <a:gd name="adj3" fmla="val 32489"/>
-            <a:gd name="adj4" fmla="val -53687"/>
+            <a:gd name="adj3" fmla="val 33095"/>
+            <a:gd name="adj4" fmla="val -135038"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -5052,9 +4539,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="85000"/>
-          </a:schemeClr>
+          <a:srgbClr val="FFFF00"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -5103,546 +4588,38 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>657411</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>74706</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>403411</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>104587</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="258" name="Line Callout 3 257"/>
+        <xdr:cNvPr id="96" name="Rectangular Callout 95"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12481111" y="11809506"/>
-          <a:ext cx="1765300" cy="563281"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout3">
+          <a:off x="8178800" y="368300"/>
+          <a:ext cx="2476500" cy="749300"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 57079"/>
-            <a:gd name="adj2" fmla="val -4017"/>
-            <a:gd name="adj3" fmla="val 57079"/>
-            <a:gd name="adj4" fmla="val -39688"/>
-            <a:gd name="adj5" fmla="val -337304"/>
-            <a:gd name="adj6" fmla="val -41218"/>
-            <a:gd name="adj7" fmla="val -964759"/>
-            <a:gd name="adj8" fmla="val -43584"/>
+            <a:gd name="adj1" fmla="val -73985"/>
+            <a:gd name="adj2" fmla="val 224750"/>
           </a:avLst>
         </a:prstGeom>
-        <a:noFill/>
         <a:ln w="38100">
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>433293</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>104588</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>164353</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>119528</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="259" name="Line Callout 2 258"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14276293" y="11839388"/>
-          <a:ext cx="1750360" cy="548340"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 48859"/>
-            <a:gd name="adj2" fmla="val 98325"/>
-            <a:gd name="adj3" fmla="val 46543"/>
-            <a:gd name="adj4" fmla="val 166901"/>
-            <a:gd name="adj5" fmla="val -758346"/>
-            <a:gd name="adj6" fmla="val 166649"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="90" name="Rectangle 89"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16903700" y="1295400"/>
-          <a:ext cx="1663700" cy="635000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(action) load account information</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="92" name="Rectangle 91"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16891000" y="2921000"/>
-          <a:ext cx="1663700" cy="635000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(action) load friend</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> list</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> information</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="93" name="Line Callout 2 92"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9194800" y="6515100"/>
-          <a:ext cx="1663700" cy="635000"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 52750"/>
-            <a:gd name="adj2" fmla="val 100827"/>
-            <a:gd name="adj3" fmla="val 50750"/>
-            <a:gd name="adj4" fmla="val 302417"/>
-            <a:gd name="adj5" fmla="val 98500"/>
-            <a:gd name="adj6" fmla="val 302188"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(action) back to album</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="94" name="Line Callout 2 93"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8826500" y="8699500"/>
-          <a:ext cx="1663700" cy="635000"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -3250"/>
-            <a:gd name="adj2" fmla="val 49682"/>
-            <a:gd name="adj3" fmla="val -217250"/>
-            <a:gd name="adj4" fmla="val 50509"/>
-            <a:gd name="adj5" fmla="val -219500"/>
-            <a:gd name="adj6" fmla="val -77201"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(action) select a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> photo</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="95" name="Line Callout 1 94"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16510000" y="7188200"/>
-          <a:ext cx="2006600" cy="469900"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout1">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 53885"/>
-            <a:gd name="adj2" fmla="val -738"/>
-            <a:gd name="adj3" fmla="val 53041"/>
-            <a:gd name="adj4" fmla="val -21244"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -5667,12 +4644,74 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(action) go to album tab</a:t>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Login </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="97" name="Rectangular Callout 96"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9613900" y="1371600"/>
+          <a:ext cx="2476500" cy="749300"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 64477"/>
+            <a:gd name="adj2" fmla="val 145089"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Login </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5971,19 +5010,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AC1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+    <sheetView topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="16" max="16" width="8.85546875" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" customWidth="1"/>
-    <col min="29" max="29" width="49.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" customWidth="1"/>
+    <col min="17" max="17" width="13.83203125" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" customWidth="1"/>
+    <col min="29" max="29" width="49.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="29:29" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="29:29" ht="19">
       <c r="AC1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5991,8 +5030,8 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6003,131 +5042,633 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="5" customWidth="1"/>
-    <col min="3" max="23" width="52.7109375" style="5" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="6.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29" style="3" customWidth="1"/>
+    <col min="3" max="3" width="54.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="39" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="5" t="s">
+    <row r="2" spans="1:6" ht="42" customHeight="1">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="5" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="8"/>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="8"/>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="8"/>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" s="6" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:A20"/>
-    <mergeCell ref="B1:B10"/>
-    <mergeCell ref="B11:B20"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="3" customWidth="1"/>
+    <col min="4" max="7" width="20.5" style="3"/>
+    <col min="8" max="8" width="10.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="3" customWidth="1"/>
+    <col min="10" max="13" width="2.6640625" style="3" customWidth="1"/>
+    <col min="14" max="15" width="2.6640625" style="4" customWidth="1"/>
+    <col min="16" max="21" width="2.6640625" style="3" customWidth="1"/>
+    <col min="22" max="16384" width="20.5" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3">
+        <v>27</v>
+      </c>
+      <c r="K1" s="3">
+        <v>28</v>
+      </c>
+      <c r="L1" s="3">
+        <v>29</v>
+      </c>
+      <c r="M1" s="3">
+        <v>30</v>
+      </c>
+      <c r="N1" s="4">
+        <v>1</v>
+      </c>
+      <c r="O1" s="4">
+        <v>2</v>
+      </c>
+      <c r="P1" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>4</v>
+      </c>
+      <c r="R1" s="3">
+        <v>5</v>
+      </c>
+      <c r="S1" s="3">
+        <v>6</v>
+      </c>
+      <c r="T1" s="3">
+        <v>7</v>
+      </c>
+      <c r="U1" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3">
+        <f>(E2+D2)/2</f>
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="5">
+        <v>42913</v>
+      </c>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:21" ht="28">
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F17" si="0">(E3+D3)/2</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="5">
+        <v>42913</v>
+      </c>
+      <c r="I3" s="5">
+        <v>42913</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="5">
+        <v>42913</v>
+      </c>
+      <c r="I4" s="5">
+        <v>42913</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="5">
+        <v>42914</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="5">
+        <v>42913</v>
+      </c>
+      <c r="I6" s="5">
+        <v>42913</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="5">
+        <v>42913</v>
+      </c>
+      <c r="I7" s="5">
+        <v>42793</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="5">
+        <v>42913</v>
+      </c>
+      <c r="I8" s="5">
+        <v>42913</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="5">
+        <v>42913</v>
+      </c>
+      <c r="I9" s="5">
+        <v>42913</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="5">
+        <v>42913</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="5">
+        <v>42915</v>
+      </c>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="5">
+        <v>42916</v>
+      </c>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3">
+        <v>4</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="5">
+        <v>42916</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="5">
+        <v>42919</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="5">
+        <v>42920</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="C16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>4</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="5">
+        <v>42921</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="5">
+        <v>42921</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8">
+      <c r="D18" s="3">
+        <f>SUM(D2:D17)</f>
+        <v>59.5</v>
+      </c>
+      <c r="E18" s="3">
+        <f>SUM(E2:E17)</f>
+        <v>68</v>
+      </c>
+      <c r="F18" s="3">
+        <f>SUM(F2:F17)</f>
+        <v>63.75</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8">
+      <c r="D19" s="3">
+        <f>D18/8</f>
+        <v>7.4375</v>
+      </c>
+      <c r="E19" s="3">
+        <f>E18/8</f>
+        <v>8.5</v>
+      </c>
+      <c r="F19" s="3">
+        <f>F18/8</f>
+        <v>7.96875</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>